<commit_message>
Add more data analysis stuffs
</commit_message>
<xml_diff>
--- a/analyses/grad-learn-compare/Data2.xlsx
+++ b/analyses/grad-learn-compare/Data2.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Files\Programming\thesis\analyses\grad-learn-compare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF33DD5-2E0C-4814-B95B-8592AE810C72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B6E56D-F11C-4E07-A3D8-E6DD7B7DDFAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{3687FE94-F347-48CF-974F-FC988C77DA1B}"/>
   </bookViews>
@@ -19,8 +19,8 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
-    <pivotCache cacheId="1" r:id="rId5"/>
+    <pivotCache cacheId="10" r:id="rId4"/>
+    <pivotCache cacheId="11" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -2545,6 +2545,917 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[Data2.xlsx]Growing Jump!PivotTable4</c:name>
+    <c:fmtId val="14"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Growing Jump'!$B$3:$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>EdgeStrategy.MIRROR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Growing Jump'!$A$5:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Growing Jump'!$B$5:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>95.696192375818626</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>112.07615451812697</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>111.36025667190516</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>93.687056223551238</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>91.035532013575022</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>93.559605662027764</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>88.614200370652156</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>84.085864118167166</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>89.6923111847467</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>78.394983070237132</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>85.722001450402246</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>89.357928088732976</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>93.376642107963406</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>104.53118234021296</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>80.203727364540015</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FE99-4619-97BC-7A0A3E85A777}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Growing Jump'!$C$3:$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>EdgeStrategy.TF_SAME</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Growing Jump'!$A$5:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Growing Jump'!$C$5:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>58.016532866160041</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>85.250057824452625</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>77.584169848759942</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>67.509972238540612</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>67.077292585372874</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>69.238542795181246</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>62.256088393075096</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>56.656640529632519</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>62.670499478067619</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>54.652424846376654</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>58.270529542650443</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>61.592332567487411</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>61.4587350572858</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>64.766808680125607</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>52.97361113343915</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FE99-4619-97BC-7A0A3E85A777}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="2032999103"/>
+        <c:axId val="1777401519"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2032999103"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1777401519"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1777401519"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2032999103"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2586,6 +3497,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3631,6 +4582,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -3676,16 +5130,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>533399</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>314324</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>176211</xdr:rowOff>
+      <xdr:rowOff>109536</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>66674</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3705,6 +5159,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>295276</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F841C7E2-997B-4333-805F-C51A9B4EAE52}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -9851,7 +11343,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2912F76A-A074-493A-A2C2-1EA0DA0C200A}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2912F76A-A074-493A-A2C2-1EA0DA0C200A}" name="PivotTable2" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="A3:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField showAll="0"/>
@@ -9926,7 +11418,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{292FE3AA-189D-49D6-A4FC-F517E5C0B8CE}" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="13">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{292FE3AA-189D-49D6-A4FC-F517E5C0B8CE}" name="PivotTable4" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="15">
   <location ref="A3:D20" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField showAll="0"/>
@@ -10040,7 +11532,7 @@
   <dataFields count="1">
     <dataField name="Average of total_seconds" fld="1" subtotal="average" baseField="4" baseItem="0"/>
   </dataFields>
-  <chartFormats count="3">
+  <chartFormats count="7">
     <chartFormat chart="12" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -10070,6 +11562,54 @@
           </reference>
           <reference field="4" count="1" selected="0">
             <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="13" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="13" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="14" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="14" format="6" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="1"/>
           </reference>
         </references>
       </pivotArea>
@@ -17836,8 +19376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6507A2E0-1FC8-46D7-971C-E356FF08E6BD}">
   <dimension ref="A3:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O33" sqref="O33"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>